<commit_message>
Update Sprint Backlog Burndown.xlsx
1) Updated sprint backlog to track progress.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c751dba731cb2a1/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{9BB774ED-A98C-AB40-8B28-581984FE53D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF190356-29D1-4D48-BDA9-98E9B744F53A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB9F85B-9B5F-4FFD-BFFE-0CF1813B788F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="22700" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7335" yWindow="-20460" windowWidth="38700" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1427,17 +1427,17 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.5" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
@@ -1473,7 +1473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1492,10 +1492,14 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1514,10 +1518,14 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1536,10 +1544,14 @@
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1558,10 +1570,14 @@
       <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1580,10 +1596,14 @@
       <c r="F7" s="2">
         <v>3</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1605,7 +1625,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1627,7 +1647,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1653,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1677,7 +1697,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1727,7 +1747,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1751,7 +1771,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1777,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1801,7 +1821,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1825,7 +1845,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1849,7 +1869,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1873,7 +1893,7 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1917,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1916,10 +1936,14 @@
       <c r="F21" s="2">
         <v>0</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1938,10 +1962,14 @@
       <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1960,10 +1988,14 @@
       <c r="F23" s="2">
         <v>0</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1982,10 +2014,14 @@
       <c r="F24" s="2">
         <v>2</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -2004,10 +2040,14 @@
       <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2026,10 +2066,14 @@
       <c r="F26" s="2">
         <v>3</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G26" s="2">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2039,7 +2083,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2049,7 +2093,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2059,7 +2103,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2069,7 +2113,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>
@@ -2087,7 +2131,7 @@
       </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H31" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Implemented Tests for the OrderPageViewModel
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c751dba731cb2a1/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{9BB774ED-A98C-AB40-8B28-581984FE53D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF190356-29D1-4D48-BDA9-98E9B744F53A}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{9BB774ED-A98C-AB40-8B28-581984FE53D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63B9F148-D80E-4DA7-BA7E-8B551ED31FFC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="22700" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="3285" windowWidth="28500" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -365,7 +365,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$31:$H$31</c:f>
+              <c:f>Sprint1!$D$31:$H$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -379,7 +379,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1427,17 +1427,17 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.5" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
@@ -1473,7 +1473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1492,10 +1492,14 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1514,10 +1518,14 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1536,10 +1544,14 @@
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1558,10 +1570,14 @@
       <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1580,10 +1596,14 @@
       <c r="F7" s="2">
         <v>3</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1602,10 +1622,14 @@
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1624,10 +1648,14 @@
       <c r="F9" s="2">
         <v>3</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1653,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1675,9 +1703,11 @@
       <c r="G11" s="2">
         <v>1</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1725,9 +1755,11 @@
       <c r="G13" s="2">
         <v>1</v>
       </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1749,9 +1781,11 @@
       <c r="G14" s="2">
         <v>2</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1777,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1799,9 +1833,11 @@
       <c r="G16" s="2">
         <v>1</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1823,9 +1859,11 @@
       <c r="G17" s="2">
         <v>1</v>
       </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1847,9 +1885,11 @@
       <c r="G18" s="2">
         <v>1</v>
       </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1871,9 +1911,11 @@
       <c r="G19" s="2">
         <v>1</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1895,9 +1937,11 @@
       <c r="G20" s="2">
         <v>1</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1916,10 +1960,14 @@
       <c r="F21" s="2">
         <v>0</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1938,10 +1986,14 @@
       <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1960,10 +2012,14 @@
       <c r="F23" s="2">
         <v>0</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1982,10 +2038,14 @@
       <c r="F24" s="2">
         <v>2</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -2004,10 +2064,14 @@
       <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G25" s="2">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2026,10 +2090,14 @@
       <c r="F26" s="2">
         <v>3</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G26" s="2">
+        <v>3</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2039,7 +2107,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2049,7 +2117,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2059,7 +2127,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2069,7 +2137,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>
@@ -2087,7 +2155,7 @@
       </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H31" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update Sprint1 Retro / Sprint2 Backlog
Update Sprint 1 Retrospective and Sprint 2 Backlog.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toruggao/Library/CloudStorage/OneDrive-Personal/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743090BE-8BF2-441A-A98F-546450459726}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4822A3CE-74D2-2B47-9813-D089390B5367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>Related User Story</t>
   </si>
@@ -199,9 +210,6 @@
     <t>Implement the Functionality to "hold" the login employee type</t>
   </si>
   <si>
-    <t>Implement the Functionality to display the current employee's information</t>
-  </si>
-  <si>
     <t>Implement Functionality to hide buttons based on the employee's role</t>
   </si>
   <si>
@@ -229,13 +237,22 @@
     <t>Assigned To</t>
   </si>
   <si>
-    <t>Improve userability through consistent sidebar navigation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Implement employee summary </t>
   </si>
   <si>
-    <t>Improve userability through changing confirmation dialogs</t>
+    <t>Vitor</t>
+  </si>
+  <si>
+    <t>Improve usability through consistent sidebar navigation</t>
+  </si>
+  <si>
+    <t>Improve usability through changing confirmation dialogs</t>
+  </si>
+  <si>
+    <t>Bugs from last sprint</t>
+  </si>
+  <si>
+    <t>Require server implementation</t>
   </si>
 </sst>
 </file>
@@ -259,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +313,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -309,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -327,6 +356,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,12 +467,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$D$27:$H$27</c:f>
+              <c:f>'Sprint 2'!$D$26:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2050,7 +2081,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2385,25 +2416,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459FC875-143C-4AA9-B6BC-6BEA6ECF23F1}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>1</v>
@@ -2418,7 +2449,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2436,16 +2467,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -2460,16 +2493,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -2484,16 +2519,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>46</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -2508,16 +2545,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -2532,16 +2571,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -2556,16 +2595,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -2580,16 +2619,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -2604,16 +2643,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -2628,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -2652,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2676,9 +2717,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -2700,13 +2741,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -2724,13 +2765,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -2748,9 +2789,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
@@ -2772,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -2796,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -2820,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2844,12 +2885,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="10" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="1">
@@ -2868,12 +2909,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="1">
@@ -2892,12 +2933,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="10" t="s">
         <v>64</v>
       </c>
       <c r="D22" s="1">
@@ -2916,16 +2957,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="2">
         <v>0</v>
@@ -2940,16 +2983,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
@@ -2964,16 +3009,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
@@ -2988,53 +3035,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="4" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="3">
-        <f>SUM(D3:D23)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
-        <f>SUM(E3:E23)</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <f>SUM(F3:F23)</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <f>SUM(G3:G23)</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <f>SUM(H3:H23)</f>
-        <v>0</v>
+      <c r="D26" s="3">
+        <f>SUM(D3:D22)</f>
+        <v>46</v>
+      </c>
+      <c r="E26" s="3">
+        <f>SUM(E3:E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f>SUM(F3:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <f>SUM(G3:G22)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <f>SUM(H3:H22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3059,14 +3092,14 @@
       <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3084,7 +3117,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -3102,7 +3135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3128,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3154,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3180,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3206,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3232,7 +3265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3258,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3284,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3310,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -3336,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3362,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3388,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3414,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3440,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3466,7 +3499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3492,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3518,7 +3551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -3544,7 +3577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3570,7 +3603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3596,7 +3629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3622,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3648,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3674,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3700,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3726,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3736,7 +3769,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3746,7 +3779,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3756,7 +3789,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3766,7 +3799,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Create server to handle request
This will allow us to send requests to the server
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743090BE-8BF2-441A-A98F-546450459726}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6358E7DB-70EA-4BE9-ABDC-95E4ADC4C8A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="495" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
@@ -441,7 +441,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2388,7 +2388,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,7 +2517,7 @@
         <v>47</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="D27" s="3">
         <f>SUM(D3:D23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
         <f>SUM(E3:E23)</f>

</xml_diff>

<commit_message>
Update the Sprint Backlog Burndown
Reflect the changes in responsibility for the server impl
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toruggao/Library/CloudStorage/OneDrive-Personal/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4822A3CE-74D2-2B47-9813-D089390B5367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90472A5F-D978-434A-9077-30A996E108A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
   <si>
     <t>Related User Story</t>
   </si>
@@ -350,14 +339,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2419,41 +2408,41 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="61.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2467,14 +2456,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="1">
@@ -2493,14 +2482,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="1">
@@ -2519,14 +2506,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D5" s="1">
@@ -2545,14 +2530,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="1">
@@ -2571,12 +2556,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="1">
@@ -2595,12 +2580,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="1">
@@ -2619,12 +2604,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="1">
@@ -2643,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -2669,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -2693,11 +2678,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>56</v>
       </c>
@@ -2717,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2741,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -2765,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
@@ -2789,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2813,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -2837,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -2861,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2885,12 +2872,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="1">
@@ -2909,12 +2896,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="1">
@@ -2933,12 +2920,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D22" s="1">
@@ -2957,11 +2944,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2983,11 +2970,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -3009,11 +2996,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -3035,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
@@ -3060,13 +3047,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3092,36 +3079,36 @@
       <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.5" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
@@ -3135,7 +3122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3161,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3187,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3213,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3239,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3265,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3291,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3317,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3343,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -3369,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3395,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3421,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3447,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3473,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3499,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3525,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3551,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -3577,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3603,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3629,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3655,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3681,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3707,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3733,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3759,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3769,7 +3756,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3779,7 +3766,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3789,7 +3776,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3799,7 +3786,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Add tests for adding component on server implementation
This will allow us to ensure that all edge cashes are considered
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6358E7DB-70EA-4BE9-ABDC-95E4ADC4C8A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105EF0C0-8121-42AD-9F61-75E58D096800}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="495" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
@@ -441,7 +441,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2388,7 +2388,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,7 +2469,7 @@
         <v>45</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -2517,7 +2517,7 @@
         <v>47</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="D27" s="3">
         <f>SUM(D3:D23)</f>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3">
         <f>SUM(E3:E23)</f>

</xml_diff>

<commit_message>
Add test cases for deleting a component
This will ensure that the edge cases for deleting a component are covered.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105EF0C0-8121-42AD-9F61-75E58D096800}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9597206-0467-4948-AC8D-F0F7817B3806}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,7 +441,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2388,7 +2388,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2493,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="D27" s="3">
         <f>SUM(D3:D23)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3">
         <f>SUM(E3:E23)</f>

</xml_diff>

<commit_message>
Updated Sprint Backlog for 3/13/24
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\SE2Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA14BDC8-10FB-4E44-AAA9-4A96CE8C0CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4E96BB-D6A3-470B-8BD1-729BABC360B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="2460" windowWidth="34200" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2416,18 +2427,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459FC875-143C-4AA9-B6BC-6BEA6ECF23F1}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2458,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2465,7 +2476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2491,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -2515,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -2539,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2565,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2589,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2613,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -2637,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -2663,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -2689,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2715,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2741,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -2765,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
@@ -2789,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2813,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -2837,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -2861,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2885,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -2909,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -2933,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -2957,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -2971,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -2983,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -3009,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -3035,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -3061,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
@@ -3085,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -3109,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="4" t="s">
         <v>8</v>
       </c>
@@ -3134,12 +3145,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>71</v>
       </c>
@@ -3166,14 +3177,14 @@
       <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3191,7 +3202,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="6"/>
       <c r="C2" s="9"/>
@@ -3209,7 +3220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3235,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3261,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3287,7 +3298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3313,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3339,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3365,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3391,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3417,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -3443,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3469,7 +3480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3495,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3521,7 +3532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3547,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3573,7 +3584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3599,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3625,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -3651,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3677,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3703,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3729,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3755,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3781,7 +3792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3807,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3833,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3843,7 +3854,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3853,7 +3864,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3863,7 +3874,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3873,7 +3884,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update Backlog to reflect the work in creating the DemoDataUtility
This is to ensure that backlog is updated with the amount of work that it took to create the DataDemoUtility for the Server Implantations
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\SE2Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380D5548-7A9E-4B90-9DC2-A9A4CBBB1373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAFE742-DAD0-452C-9A70-D954C954A26B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3615" yWindow="1380" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>Related User Story</t>
   </si>
@@ -268,6 +257,12 @@
   </si>
   <si>
     <t>Migrate Credential Manager from Local Impl to Server Impl</t>
+  </si>
+  <si>
+    <t>Create DemoData for the Server Impl</t>
+  </si>
+  <si>
+    <t>Implement a "Loading" text whenever the GUI is fetching information from the server</t>
   </si>
 </sst>
 </file>
@@ -482,24 +477,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$D$31:$H$31</c:f>
+              <c:f>'Sprint 2'!$D$33:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>77</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2096,7 +2091,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2431,20 +2426,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459FC875-143C-4AA9-B6BC-6BEA6ECF23F1}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2464,7 +2459,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2482,7 +2477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2508,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -2534,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -2560,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2586,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2612,7 +2607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2638,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -2664,70 +2659,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>5</v>
       </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
@@ -2742,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -2750,79 +2745,79 @@
         <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
         <v>4</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2">
         <v>4</v>
       </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>39</v>
@@ -2846,9 +2841,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>39</v>
@@ -2872,59 +2867,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -2932,25 +2927,25 @@
         <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -2958,57 +2953,57 @@
         <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>3</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="1">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2">
-        <v>3</v>
-      </c>
-      <c r="F21" s="2">
-        <v>3</v>
-      </c>
-      <c r="G21" s="2">
-        <v>3</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G22" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>63</v>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
@@ -3020,19 +3015,19 @@
         <v>2</v>
       </c>
       <c r="G23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
@@ -3050,15 +3045,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>68</v>
+      <c r="C25" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -3067,7 +3062,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" s="2">
         <v>0</v>
@@ -3076,68 +3071,66 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="1"/>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="1">
-        <v>3</v>
-      </c>
-      <c r="E26" s="2">
-        <v>3</v>
-      </c>
-      <c r="F26" s="2">
-        <v>3</v>
-      </c>
-      <c r="G26" s="2">
-        <v>3</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="1">
-        <v>3</v>
-      </c>
-      <c r="E27" s="2">
-        <v>2</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="D28" s="1">
         <v>3</v>
       </c>
@@ -3148,13 +3141,13 @@
         <v>3</v>
       </c>
       <c r="G28" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -3162,16 +3155,16 @@
         <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1">
         <v>3</v>
       </c>
       <c r="E29" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2">
         <v>0</v>
@@ -3180,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
@@ -3188,56 +3181,108 @@
         <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2">
+        <v>3</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3</v>
+      </c>
+      <c r="F31" s="2">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="1">
-        <v>3</v>
-      </c>
-      <c r="E30" s="2">
-        <v>3</v>
-      </c>
-      <c r="F30" s="2">
-        <v>2</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="4" t="s">
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3</v>
+      </c>
+      <c r="F32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="3">
-        <f>SUM(D3:D24)</f>
-        <v>77</v>
-      </c>
-      <c r="E31" s="3">
-        <f>SUM(E3:E24)</f>
-        <v>69</v>
-      </c>
-      <c r="F31" s="3">
-        <f>SUM(F3:F24)</f>
-        <v>60</v>
-      </c>
-      <c r="G31" s="3">
-        <f>SUM(G3:G24)</f>
-        <v>19</v>
-      </c>
-      <c r="H31" s="3">
-        <f>SUM(H3:H24)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="D33" s="3">
+        <f>SUM(D3:D26)</f>
+        <v>80</v>
+      </c>
+      <c r="E33" s="3">
+        <f>SUM(E3:E26)</f>
+        <v>72</v>
+      </c>
+      <c r="F33" s="3">
+        <f>SUM(F3:F26)</f>
+        <v>63</v>
+      </c>
+      <c r="G33" s="3">
+        <f>SUM(G3:G26)</f>
+        <v>22</v>
+      </c>
+      <c r="H33" s="3">
+        <f>SUM(H3:H26)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="8" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3263,14 +3308,14 @@
       <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.3984375" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3288,7 +3333,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="9"/>
       <c r="B2" s="6"/>
       <c r="C2" s="9"/>
@@ -3306,7 +3351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3332,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3358,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3384,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3410,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3436,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3462,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3488,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3514,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -3540,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3566,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3592,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3618,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3644,7 +3689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3670,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3696,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3722,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -3748,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3774,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3800,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3826,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3852,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3878,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3904,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3930,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3940,7 +3985,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3950,7 +3995,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3960,7 +4005,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3970,7 +4015,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update Sprint Backlog to reflect tests for the server side
This will ensure that all the functionality is working on the server
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAFE742-DAD0-452C-9A70-D954C954A26B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1673D0-EF80-4B1D-8385-17A5040F0D0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3615" yWindow="1380" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="83">
   <si>
     <t>Related User Story</t>
   </si>
@@ -263,6 +263,18 @@
   </si>
   <si>
     <t>Implement a "Loading" text whenever the GUI is fetching information from the server</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Implement Tests for the Components Server Side</t>
+  </si>
+  <si>
+    <t>Implement Tests for the Products Server Side</t>
+  </si>
+  <si>
+    <t>Implement Tests for the Orders Server Side</t>
   </si>
 </sst>
 </file>
@@ -477,7 +489,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$D$33:$H$33</c:f>
+              <c:f>'Sprint 2'!$D$36:$H$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2426,20 +2438,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459FC875-143C-4AA9-B6BC-6BEA6ECF23F1}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2459,7 +2471,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2477,7 +2489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2503,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -2529,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -2555,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2581,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2607,7 +2619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2633,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -2659,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -2685,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2711,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2737,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -2763,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -2789,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2815,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2841,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2867,7 +2879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -2893,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2919,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -2945,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -2971,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -2997,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -3021,7 +3033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -3045,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -3071,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -3095,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -3121,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -3173,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
@@ -3199,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
@@ -3225,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -3251,38 +3263,110 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C33" s="4" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1">
+        <v>3</v>
+      </c>
+      <c r="H34" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D36" s="3">
         <f>SUM(D3:D26)</f>
         <v>80</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E36" s="3">
         <f>SUM(E3:E26)</f>
         <v>72</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F36" s="3">
         <f>SUM(F3:F26)</f>
         <v>63</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G36" s="3">
         <f>SUM(G3:G26)</f>
         <v>22</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H36" s="3">
         <f>SUM(H3:H26)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" s="7" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="8" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3308,14 +3392,14 @@
       <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.3984375" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3333,7 +3417,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="6"/>
       <c r="C2" s="9"/>
@@ -3351,7 +3435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3377,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3403,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3429,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3455,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3481,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3507,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3533,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3559,7 +3643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -3585,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3611,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3637,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3663,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3689,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3715,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3741,7 +3825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3767,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -3793,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3819,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3845,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3871,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3897,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3923,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3949,7 +4033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3975,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3985,7 +4069,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3995,7 +4079,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4005,7 +4089,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4015,7 +4099,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update Use Case Scenarios
Update the use scenarios to reflect the current application logic from the last sprint
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\SE2Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAEFC92-B7D1-4D4E-98D4-1F2DD5142B4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C2EC4-B251-4E7B-8C22-33F765AB6468}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1380" windowWidth="28800" windowHeight="15350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3623" yWindow="1380" windowWidth="28800" windowHeight="15353" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
   <si>
     <t>Related User Story</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>Create DemoData for the Server Impl</t>
-  </si>
-  <si>
-    <t>Implement a "Loading" text whenever the GUI is fetching information from the server</t>
   </si>
   <si>
     <t>Server</t>
@@ -483,24 +480,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$D$34:$H$34</c:f>
+              <c:f>'Sprint 2'!$D$33:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>74</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2432,20 +2429,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459FC875-143C-4AA9-B6BC-6BEA6ECF23F1}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2465,7 +2462,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2483,7 +2480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2509,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -2535,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -2561,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2587,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2610,10 +2607,10 @@
         <v>2</v>
       </c>
       <c r="H7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2639,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -2665,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -2691,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2717,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2743,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -2769,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -2795,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2821,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2847,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2873,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -2899,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2925,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -2951,13 +2948,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>76</v>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -2969,19 +2968,21 @@
         <v>2</v>
       </c>
       <c r="G21" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C22" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
@@ -2999,15 +3000,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
@@ -3025,13 +3026,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="8" t="s">
-        <v>62</v>
+      <c r="B24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
@@ -3040,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2">
         <v>0</v>
@@ -3049,59 +3052,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G25" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D26" s="1">
         <v>3</v>
       </c>
       <c r="E26" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
@@ -3109,16 +3112,16 @@
         <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1">
         <v>3</v>
       </c>
       <c r="E27" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G27" s="2">
         <v>0</v>
@@ -3127,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -3135,7 +3138,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D28" s="1">
         <v>3</v>
@@ -3144,7 +3147,7 @@
         <v>3</v>
       </c>
       <c r="F28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G28" s="2">
         <v>0</v>
@@ -3153,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1">
         <v>3</v>
@@ -3179,38 +3182,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>71</v>
+      <c r="C30" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="D30" s="1">
         <v>3</v>
       </c>
-      <c r="E30" s="2">
-        <v>3</v>
-      </c>
-      <c r="F30" s="2">
-        <v>2</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>78</v>
@@ -3231,12 +3234,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>79</v>
@@ -3257,64 +3260,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="1">
-        <v>3</v>
-      </c>
-      <c r="E33" s="1">
-        <v>3</v>
-      </c>
-      <c r="F33" s="1">
-        <v>3</v>
-      </c>
-      <c r="G33" s="1">
-        <v>2</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C34" s="4" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="3">
-        <f>SUM(D3:D24)</f>
-        <v>74</v>
-      </c>
-      <c r="E34" s="3">
-        <f>SUM(E3:E24)</f>
-        <v>66</v>
-      </c>
-      <c r="F34" s="3">
-        <f>SUM(F3:F24)</f>
-        <v>57</v>
-      </c>
-      <c r="G34" s="3">
-        <f>SUM(G3:G24)</f>
-        <v>16</v>
-      </c>
-      <c r="H34" s="3">
-        <f>SUM(H3:H24)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
+      <c r="D33" s="3">
+        <f>SUM(D3:D23)</f>
+        <v>72</v>
+      </c>
+      <c r="E33" s="3">
+        <f>SUM(E3:E23)</f>
+        <v>64</v>
+      </c>
+      <c r="F33" s="3">
+        <f>SUM(F3:F23)</f>
+        <v>55</v>
+      </c>
+      <c r="G33" s="3">
+        <f>SUM(G3:G23)</f>
+        <v>14</v>
+      </c>
+      <c r="H33" s="3">
+        <f>SUM(H3:H23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="8" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3340,14 +3317,14 @@
       <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.46484375" customWidth="1"/>
+    <col min="4" max="4" width="14.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3365,7 +3342,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="9"/>
       <c r="B2" s="6"/>
       <c r="C2" s="9"/>
@@ -3383,7 +3360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3409,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3435,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3461,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3487,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3513,7 +3490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3539,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3565,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3591,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -3617,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3643,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3669,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3695,7 +3672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3721,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3747,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3773,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3799,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -3825,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3851,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3877,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3903,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3929,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3955,7 +3932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3981,7 +3958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -4007,7 +3984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -4017,7 +3994,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4027,7 +4004,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4037,7 +4014,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4047,7 +4024,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update Spring Backlog Burndown
Update the sprint backlog to reflect the items that are due for Sprint 3
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C2EC4-B251-4E7B-8C22-33F765AB6468}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767AB0A1-33D9-454D-B103-282F3A118B8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3623" yWindow="1380" windowWidth="28800" windowHeight="15353" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="1380" windowWidth="28800" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
-    <sheet name="Sprint1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sprint1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="93">
   <si>
     <t>Related User Story</t>
   </si>
@@ -266,6 +267,45 @@
   </si>
   <si>
     <t>Implement Tests for the Orders Server Side</t>
+  </si>
+  <si>
+    <t>Style the login view</t>
+  </si>
+  <si>
+    <t>Style the home view</t>
+  </si>
+  <si>
+    <t>Style the inventory view</t>
+  </si>
+  <si>
+    <t>Style the add component view</t>
+  </si>
+  <si>
+    <t>Style the edit component view</t>
+  </si>
+  <si>
+    <t>Style the add product view</t>
+  </si>
+  <si>
+    <t>Style the edit product view</t>
+  </si>
+  <si>
+    <t>Style the edit credential view</t>
+  </si>
+  <si>
+    <t>Style the register view</t>
+  </si>
+  <si>
+    <t>Style the order view</t>
+  </si>
+  <si>
+    <t>Update the search product to search as the user is typing</t>
+  </si>
+  <si>
+    <t>Update the search component to search as the user is typing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Alerts When Stock is Low </t>
   </si>
 </sst>
 </file>
@@ -351,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -371,6 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,6 +430,297 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$D$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-830C-4928-8093-D07C837FD033}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="567059032"/>
+        <c:axId val="567059360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="567059032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="567059360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="567059360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="567059032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -679,7 +1011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1050,6 +1382,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2082,7 +2454,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFADE74C-2964-4AF3-A747-453DB6BEE0FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2125,7 +3056,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2428,21 +3359,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459FC875-143C-4AA9-B6BC-6BEA6ECF23F1}">
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E094ACB9-BBC8-4B29-B99D-6CB66C10CDCA}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2462,7 +3393,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2480,11 +3411,429 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <f>SUM(D3:D15)</f>
+        <v>19</v>
+      </c>
+      <c r="E16" s="3">
+        <f>SUM(E3:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <f>SUM(F3:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <f>SUM(G3:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <f>SUM(H3:H15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459FC875-143C-4AA9-B6BC-6BEA6ECF23F1}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2506,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -2532,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -2558,7 +3907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2584,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2610,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2636,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -2662,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -2688,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2714,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2740,7 +4089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -2766,7 +4115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -2792,7 +4141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2818,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2844,7 +4193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2870,7 +4219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -2896,7 +4245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2922,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -2948,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -2974,7 +4323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -3000,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -3026,7 +4375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -3052,7 +4401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -3078,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -3104,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
@@ -3130,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -3156,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -3182,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
@@ -3208,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
@@ -3234,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
@@ -3260,7 +4609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>8</v>
       </c>
@@ -3285,12 +4634,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>69</v>
       </c>
@@ -3309,7 +4658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -3317,14 +4666,14 @@
       <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.46484375" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3342,7 +4691,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="6"/>
       <c r="C2" s="9"/>
@@ -3360,7 +4709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3386,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3412,7 +4761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3438,7 +4787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3464,7 +4813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3490,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3516,7 +4865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3542,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3568,7 +4917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -3594,7 +4943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3620,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3646,7 +4995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3672,7 +5021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3698,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3724,7 +5073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3750,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3776,7 +5125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -3802,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3828,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3854,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3880,7 +5229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3906,7 +5255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -3932,7 +5281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3958,7 +5307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -3984,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3994,7 +5343,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4004,7 +5353,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4014,7 +5363,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4024,7 +5373,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>